<commit_message>
commit new oracle folder
</commit_message>
<xml_diff>
--- a/Oracle_Knowledge_Links.xlsx
+++ b/Oracle_Knowledge_Links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabya\gitrepos\oracle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2980D896-0B10-4197-B8A3-C80B359EBF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E409073C-ED47-4D52-9ACC-FB940D555436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{21D15681-6EA7-4197-97B9-FD00DBE7A6A9}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="729">
   <si>
     <t>Serial No</t>
   </si>
@@ -2205,6 +2205,15 @@
   </si>
   <si>
     <t>SQL*Plus access without an OS login</t>
+  </si>
+  <si>
+    <t>AskTom Blogs</t>
+  </si>
+  <si>
+    <t>Edition-Based Redefinition, Part 2</t>
+  </si>
+  <si>
+    <t>https://asktom.oracle.com/Misc/oramag/edition-based-redefinition-part-2.html</t>
   </si>
 </sst>
 </file>
@@ -2404,13 +2413,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A329D12-82F4-48CA-B6A5-FC44496504A4}" name="Table1" displayName="Table1" ref="A1:F335" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
-  <autoFilter ref="A1:F335" xr:uid="{3A329D12-82F4-48CA-B6A5-FC44496504A4}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Jeff Smith Blog"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C54AE5A3-6185-4B4A-8944-4DD06AF2943B}" name="Serial No"/>
     <tableColumn id="2" xr3:uid="{B804B430-797F-47D9-8692-E8681C88043E}" name="SOURCE"/>
@@ -2734,11 +2736,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9EE77A-69C7-4F38-9C2C-6F33C504A344}">
-  <dimension ref="A1:F335"/>
+  <dimension ref="A1:F281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F336" sqref="F336"/>
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F284" sqref="F284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2771,7 +2773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2791,7 +2793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2811,7 +2813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2831,7 +2833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2851,7 +2853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2871,7 +2873,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2891,7 +2893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2911,7 +2913,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2931,7 +2933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2951,7 +2953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2971,7 +2973,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2991,7 +2993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3011,7 +3013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3031,7 +3033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3051,7 +3053,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3071,7 +3073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3091,7 +3093,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3111,7 +3113,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3131,7 +3133,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3171,7 +3173,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3191,7 +3193,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3211,7 +3213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3231,7 +3233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3251,7 +3253,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3271,7 +3273,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3291,7 +3293,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3311,7 +3313,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3331,7 +3333,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3351,7 +3353,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3371,7 +3373,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3391,7 +3393,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3411,7 +3413,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3431,7 +3433,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3451,7 +3453,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3471,7 +3473,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3491,7 +3493,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3511,7 +3513,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3531,7 +3533,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3551,7 +3553,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3571,7 +3573,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3591,7 +3593,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3611,7 +3613,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3631,7 +3633,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3651,7 +3653,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3671,7 +3673,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3691,7 +3693,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3711,7 +3713,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3731,7 +3733,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3751,7 +3753,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3771,7 +3773,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3791,7 +3793,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3811,7 +3813,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3831,7 +3833,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3851,7 +3853,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3871,7 +3873,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3891,7 +3893,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3911,7 +3913,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3931,7 +3933,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3951,7 +3953,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3971,7 +3973,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3991,7 +3993,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4011,7 +4013,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4031,7 +4033,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4051,7 +4053,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4071,7 +4073,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4091,7 +4093,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4111,7 +4113,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4131,7 +4133,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4171,7 +4173,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4191,7 +4193,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4211,7 +4213,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4231,7 +4233,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4251,7 +4253,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4271,7 +4273,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4291,7 +4293,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4311,7 +4313,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4331,7 +4333,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4351,7 +4353,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4371,7 +4373,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4391,7 +4393,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4411,7 +4413,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4431,7 +4433,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4451,7 +4453,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4471,7 +4473,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4491,7 +4493,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4511,7 +4513,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4531,7 +4533,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4551,7 +4553,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4571,7 +4573,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4591,7 +4593,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4611,7 +4613,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4631,7 +4633,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4651,7 +4653,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4671,7 +4673,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4691,7 +4693,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4711,7 +4713,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4731,7 +4733,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4751,7 +4753,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4771,7 +4773,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4791,7 +4793,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4811,7 +4813,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4831,7 +4833,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4891,7 +4893,10 @@
         <v>277</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>107</v>
+      </c>
       <c r="B108" t="s">
         <v>280</v>
       </c>
@@ -4908,7 +4913,10 @@
         <v>282</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>108</v>
+      </c>
       <c r="B109" t="s">
         <v>251</v>
       </c>
@@ -4925,7 +4933,10 @@
         <v>284</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>109</v>
+      </c>
       <c r="B110" t="s">
         <v>251</v>
       </c>
@@ -4942,7 +4953,10 @@
         <v>258</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>110</v>
+      </c>
       <c r="B111" t="s">
         <v>251</v>
       </c>
@@ -4959,7 +4973,10 @@
         <v>286</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>111</v>
+      </c>
       <c r="B112" t="s">
         <v>50</v>
       </c>
@@ -4976,7 +4993,10 @@
         <v>288</v>
       </c>
     </row>
-    <row r="113" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>112</v>
+      </c>
       <c r="B113" t="s">
         <v>291</v>
       </c>
@@ -4993,7 +5013,10 @@
         <v>290</v>
       </c>
     </row>
-    <row r="114" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>113</v>
+      </c>
       <c r="B114" t="s">
         <v>50</v>
       </c>
@@ -5010,7 +5033,10 @@
         <v>292</v>
       </c>
     </row>
-    <row r="115" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>114</v>
+      </c>
       <c r="B115" t="s">
         <v>50</v>
       </c>
@@ -5027,7 +5053,10 @@
         <v>299</v>
       </c>
     </row>
-    <row r="116" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>115</v>
+      </c>
       <c r="B116" t="s">
         <v>251</v>
       </c>
@@ -5044,7 +5073,10 @@
         <v>341</v>
       </c>
     </row>
-    <row r="117" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>116</v>
+      </c>
       <c r="B117" t="s">
         <v>251</v>
       </c>
@@ -5061,7 +5093,10 @@
         <v>302</v>
       </c>
     </row>
-    <row r="118" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>117</v>
+      </c>
       <c r="B118" t="s">
         <v>251</v>
       </c>
@@ -5078,7 +5113,10 @@
         <v>304</v>
       </c>
     </row>
-    <row r="119" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>118</v>
+      </c>
       <c r="B119" t="s">
         <v>307</v>
       </c>
@@ -5095,7 +5133,10 @@
         <v>306</v>
       </c>
     </row>
-    <row r="120" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>119</v>
+      </c>
       <c r="B120" t="s">
         <v>307</v>
       </c>
@@ -5109,9 +5150,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="121" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>120</v>
+      </c>
       <c r="B121" t="s">
-        <v>230</v>
+        <v>726</v>
       </c>
       <c r="C121" t="s">
         <v>5</v>
@@ -5126,7 +5170,10 @@
         <v>311</v>
       </c>
     </row>
-    <row r="122" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>121</v>
+      </c>
       <c r="B122" t="s">
         <v>145</v>
       </c>
@@ -5143,7 +5190,10 @@
         <v>312</v>
       </c>
     </row>
-    <row r="123" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>122</v>
+      </c>
       <c r="B123" t="s">
         <v>251</v>
       </c>
@@ -5160,7 +5210,10 @@
         <v>314</v>
       </c>
     </row>
-    <row r="124" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>123</v>
+      </c>
       <c r="B124" t="s">
         <v>251</v>
       </c>
@@ -5177,7 +5230,10 @@
         <v>343</v>
       </c>
     </row>
-    <row r="125" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>124</v>
+      </c>
       <c r="B125" t="s">
         <v>251</v>
       </c>
@@ -5194,7 +5250,10 @@
         <v>345</v>
       </c>
     </row>
-    <row r="126" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>125</v>
+      </c>
       <c r="B126" t="s">
         <v>251</v>
       </c>
@@ -5211,7 +5270,10 @@
         <v>347</v>
       </c>
     </row>
-    <row r="127" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>126</v>
+      </c>
       <c r="B127" t="s">
         <v>230</v>
       </c>
@@ -5228,7 +5290,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="128" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>127</v>
+      </c>
       <c r="B128" t="s">
         <v>230</v>
       </c>
@@ -5245,7 +5310,10 @@
         <v>361</v>
       </c>
     </row>
-    <row r="129" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>128</v>
+      </c>
       <c r="B129" t="s">
         <v>230</v>
       </c>
@@ -5262,7 +5330,10 @@
         <v>359</v>
       </c>
     </row>
-    <row r="130" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>129</v>
+      </c>
       <c r="B130" t="s">
         <v>230</v>
       </c>
@@ -5279,7 +5350,10 @@
         <v>357</v>
       </c>
     </row>
-    <row r="131" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>130</v>
+      </c>
       <c r="B131" t="s">
         <v>230</v>
       </c>
@@ -5296,7 +5370,10 @@
         <v>355</v>
       </c>
     </row>
-    <row r="132" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>131</v>
+      </c>
       <c r="B132" t="s">
         <v>230</v>
       </c>
@@ -5313,7 +5390,10 @@
         <v>353</v>
       </c>
     </row>
-    <row r="133" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>132</v>
+      </c>
       <c r="B133" t="s">
         <v>230</v>
       </c>
@@ -5330,7 +5410,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="134" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>133</v>
+      </c>
       <c r="B134" t="s">
         <v>230</v>
       </c>
@@ -5347,7 +5430,10 @@
         <v>348</v>
       </c>
     </row>
-    <row r="135" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>134</v>
+      </c>
       <c r="B135" t="s">
         <v>230</v>
       </c>
@@ -5364,7 +5450,10 @@
         <v>365</v>
       </c>
     </row>
-    <row r="136" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>135</v>
+      </c>
       <c r="B136" t="s">
         <v>230</v>
       </c>
@@ -5381,7 +5470,10 @@
         <v>368</v>
       </c>
     </row>
-    <row r="137" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>136</v>
+      </c>
       <c r="B137" t="s">
         <v>230</v>
       </c>
@@ -5398,7 +5490,10 @@
         <v>371</v>
       </c>
     </row>
-    <row r="138" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>137</v>
+      </c>
       <c r="B138" t="s">
         <v>230</v>
       </c>
@@ -5415,7 +5510,10 @@
         <v>373</v>
       </c>
     </row>
-    <row r="139" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>138</v>
+      </c>
       <c r="B139" t="s">
         <v>230</v>
       </c>
@@ -5432,7 +5530,10 @@
         <v>375</v>
       </c>
     </row>
-    <row r="140" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>139</v>
+      </c>
       <c r="B140" t="s">
         <v>230</v>
       </c>
@@ -5449,7 +5550,10 @@
         <v>378</v>
       </c>
     </row>
-    <row r="141" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>140</v>
+      </c>
       <c r="B141" t="s">
         <v>230</v>
       </c>
@@ -5466,7 +5570,10 @@
         <v>380</v>
       </c>
     </row>
-    <row r="142" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>141</v>
+      </c>
       <c r="B142" t="s">
         <v>230</v>
       </c>
@@ -5483,7 +5590,10 @@
         <v>383</v>
       </c>
     </row>
-    <row r="143" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>142</v>
+      </c>
       <c r="B143" t="s">
         <v>230</v>
       </c>
@@ -5500,7 +5610,10 @@
         <v>385</v>
       </c>
     </row>
-    <row r="144" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>143</v>
+      </c>
       <c r="B144" t="s">
         <v>230</v>
       </c>
@@ -5517,7 +5630,10 @@
         <v>388</v>
       </c>
     </row>
-    <row r="145" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>144</v>
+      </c>
       <c r="B145" t="s">
         <v>230</v>
       </c>
@@ -5534,7 +5650,10 @@
         <v>390</v>
       </c>
     </row>
-    <row r="146" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>145</v>
+      </c>
       <c r="B146" t="s">
         <v>230</v>
       </c>
@@ -5551,7 +5670,10 @@
         <v>393</v>
       </c>
     </row>
-    <row r="147" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>146</v>
+      </c>
       <c r="B147" t="s">
         <v>230</v>
       </c>
@@ -5568,7 +5690,10 @@
         <v>395</v>
       </c>
     </row>
-    <row r="148" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>147</v>
+      </c>
       <c r="B148" t="s">
         <v>230</v>
       </c>
@@ -5585,7 +5710,10 @@
         <v>397</v>
       </c>
     </row>
-    <row r="149" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>148</v>
+      </c>
       <c r="B149" t="s">
         <v>230</v>
       </c>
@@ -5602,7 +5730,10 @@
         <v>400</v>
       </c>
     </row>
-    <row r="150" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>149</v>
+      </c>
       <c r="B150" t="s">
         <v>230</v>
       </c>
@@ -5619,7 +5750,10 @@
         <v>401</v>
       </c>
     </row>
-    <row r="151" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>150</v>
+      </c>
       <c r="B151" t="s">
         <v>230</v>
       </c>
@@ -5636,7 +5770,10 @@
         <v>404</v>
       </c>
     </row>
-    <row r="152" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>151</v>
+      </c>
       <c r="B152" t="s">
         <v>230</v>
       </c>
@@ -5653,7 +5790,10 @@
         <v>407</v>
       </c>
     </row>
-    <row r="153" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>152</v>
+      </c>
       <c r="B153" t="s">
         <v>230</v>
       </c>
@@ -5670,7 +5810,10 @@
         <v>409</v>
       </c>
     </row>
-    <row r="154" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>153</v>
+      </c>
       <c r="B154" t="s">
         <v>230</v>
       </c>
@@ -5687,7 +5830,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="155" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>154</v>
+      </c>
       <c r="B155" t="s">
         <v>230</v>
       </c>
@@ -5704,7 +5850,10 @@
         <v>413</v>
       </c>
     </row>
-    <row r="156" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>155</v>
+      </c>
       <c r="B156" t="s">
         <v>230</v>
       </c>
@@ -5721,7 +5870,10 @@
         <v>416</v>
       </c>
     </row>
-    <row r="157" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>156</v>
+      </c>
       <c r="B157" t="s">
         <v>230</v>
       </c>
@@ -5738,7 +5890,10 @@
         <v>418</v>
       </c>
     </row>
-    <row r="158" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>157</v>
+      </c>
       <c r="B158" t="s">
         <v>230</v>
       </c>
@@ -5755,7 +5910,10 @@
         <v>420</v>
       </c>
     </row>
-    <row r="159" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>158</v>
+      </c>
       <c r="B159" t="s">
         <v>230</v>
       </c>
@@ -5772,7 +5930,10 @@
         <v>422</v>
       </c>
     </row>
-    <row r="160" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>159</v>
+      </c>
       <c r="B160" t="s">
         <v>230</v>
       </c>
@@ -5789,7 +5950,10 @@
         <v>424</v>
       </c>
     </row>
-    <row r="161" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>160</v>
+      </c>
       <c r="B161" t="s">
         <v>230</v>
       </c>
@@ -5806,7 +5970,10 @@
         <v>427</v>
       </c>
     </row>
-    <row r="162" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>161</v>
+      </c>
       <c r="B162" t="s">
         <v>230</v>
       </c>
@@ -5823,7 +5990,10 @@
         <v>373</v>
       </c>
     </row>
-    <row r="163" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>162</v>
+      </c>
       <c r="B163" t="s">
         <v>230</v>
       </c>
@@ -5840,7 +6010,10 @@
         <v>380</v>
       </c>
     </row>
-    <row r="164" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>163</v>
+      </c>
       <c r="B164" t="s">
         <v>230</v>
       </c>
@@ -5857,7 +6030,10 @@
         <v>430</v>
       </c>
     </row>
-    <row r="165" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>164</v>
+      </c>
       <c r="B165" t="s">
         <v>230</v>
       </c>
@@ -5874,7 +6050,10 @@
         <v>432</v>
       </c>
     </row>
-    <row r="166" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>165</v>
+      </c>
       <c r="B166" t="s">
         <v>230</v>
       </c>
@@ -5891,7 +6070,10 @@
         <v>433</v>
       </c>
     </row>
-    <row r="167" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>166</v>
+      </c>
       <c r="B167" t="s">
         <v>230</v>
       </c>
@@ -5908,7 +6090,10 @@
         <v>390</v>
       </c>
     </row>
-    <row r="168" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>167</v>
+      </c>
       <c r="B168" t="s">
         <v>230</v>
       </c>
@@ -5925,7 +6110,10 @@
         <v>383</v>
       </c>
     </row>
-    <row r="169" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>168</v>
+      </c>
       <c r="B169" t="s">
         <v>230</v>
       </c>
@@ -5942,7 +6130,10 @@
         <v>437</v>
       </c>
     </row>
-    <row r="170" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>169</v>
+      </c>
       <c r="B170" t="s">
         <v>230</v>
       </c>
@@ -5959,7 +6150,10 @@
         <v>397</v>
       </c>
     </row>
-    <row r="171" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>170</v>
+      </c>
       <c r="B171" t="s">
         <v>230</v>
       </c>
@@ -5976,7 +6170,10 @@
         <v>439</v>
       </c>
     </row>
-    <row r="172" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>171</v>
+      </c>
       <c r="B172" t="s">
         <v>230</v>
       </c>
@@ -5993,7 +6190,10 @@
         <v>441</v>
       </c>
     </row>
-    <row r="173" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>172</v>
+      </c>
       <c r="B173" t="s">
         <v>230</v>
       </c>
@@ -6010,7 +6210,10 @@
         <v>443</v>
       </c>
     </row>
-    <row r="174" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>173</v>
+      </c>
       <c r="B174" t="s">
         <v>230</v>
       </c>
@@ -6027,7 +6230,10 @@
         <v>445</v>
       </c>
     </row>
-    <row r="175" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>174</v>
+      </c>
       <c r="B175" t="s">
         <v>230</v>
       </c>
@@ -6044,7 +6250,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="176" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>175</v>
+      </c>
       <c r="B176" t="s">
         <v>230</v>
       </c>
@@ -6061,7 +6270,10 @@
         <v>448</v>
       </c>
     </row>
-    <row r="177" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>176</v>
+      </c>
       <c r="B177" t="s">
         <v>452</v>
       </c>
@@ -6078,7 +6290,10 @@
         <v>451</v>
       </c>
     </row>
-    <row r="178" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>177</v>
+      </c>
       <c r="B178" t="s">
         <v>454</v>
       </c>
@@ -6095,7 +6310,10 @@
         <v>455</v>
       </c>
     </row>
-    <row r="179" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>178</v>
+      </c>
       <c r="B179" t="s">
         <v>145</v>
       </c>
@@ -6112,7 +6330,10 @@
         <v>589</v>
       </c>
     </row>
-    <row r="180" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>179</v>
+      </c>
       <c r="B180" t="s">
         <v>230</v>
       </c>
@@ -6129,7 +6350,10 @@
         <v>457</v>
       </c>
     </row>
-    <row r="181" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>180</v>
+      </c>
       <c r="B181" t="s">
         <v>230</v>
       </c>
@@ -6146,7 +6370,10 @@
         <v>460</v>
       </c>
     </row>
-    <row r="182" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>181</v>
+      </c>
       <c r="B182" t="s">
         <v>230</v>
       </c>
@@ -6163,7 +6390,10 @@
         <v>462</v>
       </c>
     </row>
-    <row r="183" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>182</v>
+      </c>
       <c r="B183" t="s">
         <v>230</v>
       </c>
@@ -6180,7 +6410,10 @@
         <v>464</v>
       </c>
     </row>
-    <row r="184" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>183</v>
+      </c>
       <c r="B184" t="s">
         <v>230</v>
       </c>
@@ -6197,7 +6430,10 @@
         <v>353</v>
       </c>
     </row>
-    <row r="185" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>184</v>
+      </c>
       <c r="B185" t="s">
         <v>50</v>
       </c>
@@ -6214,7 +6450,10 @@
         <v>466</v>
       </c>
     </row>
-    <row r="186" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>185</v>
+      </c>
       <c r="B186" t="s">
         <v>230</v>
       </c>
@@ -6231,7 +6470,10 @@
         <v>469</v>
       </c>
     </row>
-    <row r="187" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>186</v>
+      </c>
       <c r="B187" t="s">
         <v>230</v>
       </c>
@@ -6248,7 +6490,10 @@
         <v>471</v>
       </c>
     </row>
-    <row r="188" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>187</v>
+      </c>
       <c r="B188" t="s">
         <v>454</v>
       </c>
@@ -6265,7 +6510,10 @@
         <v>473</v>
       </c>
     </row>
-    <row r="189" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>188</v>
+      </c>
       <c r="B189" t="s">
         <v>454</v>
       </c>
@@ -6282,7 +6530,10 @@
         <v>475</v>
       </c>
     </row>
-    <row r="190" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>189</v>
+      </c>
       <c r="B190" t="s">
         <v>454</v>
       </c>
@@ -6299,7 +6550,10 @@
         <v>477</v>
       </c>
     </row>
-    <row r="191" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>190</v>
+      </c>
       <c r="B191" t="s">
         <v>454</v>
       </c>
@@ -6316,7 +6570,10 @@
         <v>479</v>
       </c>
     </row>
-    <row r="192" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>191</v>
+      </c>
       <c r="B192" t="s">
         <v>454</v>
       </c>
@@ -6333,7 +6590,10 @@
         <v>481</v>
       </c>
     </row>
-    <row r="193" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>192</v>
+      </c>
       <c r="B193" t="s">
         <v>454</v>
       </c>
@@ -6350,7 +6610,10 @@
         <v>483</v>
       </c>
     </row>
-    <row r="194" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>193</v>
+      </c>
       <c r="B194" t="s">
         <v>485</v>
       </c>
@@ -6367,7 +6630,10 @@
         <v>486</v>
       </c>
     </row>
-    <row r="195" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>194</v>
+      </c>
       <c r="B195" t="s">
         <v>488</v>
       </c>
@@ -6384,7 +6650,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="196" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>195</v>
+      </c>
       <c r="B196" t="s">
         <v>488</v>
       </c>
@@ -6401,7 +6670,10 @@
         <v>492</v>
       </c>
     </row>
-    <row r="197" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>196</v>
+      </c>
       <c r="B197" t="s">
         <v>230</v>
       </c>
@@ -6418,7 +6690,10 @@
         <v>495</v>
       </c>
     </row>
-    <row r="198" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>197</v>
+      </c>
       <c r="B198" t="s">
         <v>230</v>
       </c>
@@ -6435,7 +6710,10 @@
         <v>497</v>
       </c>
     </row>
-    <row r="199" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>198</v>
+      </c>
       <c r="B199" t="s">
         <v>499</v>
       </c>
@@ -6452,7 +6730,10 @@
         <v>500</v>
       </c>
     </row>
-    <row r="200" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>199</v>
+      </c>
       <c r="B200" t="s">
         <v>502</v>
       </c>
@@ -6469,7 +6750,10 @@
         <v>504</v>
       </c>
     </row>
-    <row r="201" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>200</v>
+      </c>
       <c r="B201" t="s">
         <v>502</v>
       </c>
@@ -6486,7 +6770,10 @@
         <v>506</v>
       </c>
     </row>
-    <row r="202" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>201</v>
+      </c>
       <c r="B202" t="s">
         <v>499</v>
       </c>
@@ -6503,7 +6790,10 @@
         <v>508</v>
       </c>
     </row>
-    <row r="203" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>202</v>
+      </c>
       <c r="B203" t="s">
         <v>499</v>
       </c>
@@ -6520,7 +6810,10 @@
         <v>510</v>
       </c>
     </row>
-    <row r="204" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>203</v>
+      </c>
       <c r="B204" t="s">
         <v>230</v>
       </c>
@@ -6537,7 +6830,10 @@
         <v>513</v>
       </c>
     </row>
-    <row r="205" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>204</v>
+      </c>
       <c r="B205" t="s">
         <v>251</v>
       </c>
@@ -6554,7 +6850,10 @@
         <v>515</v>
       </c>
     </row>
-    <row r="206" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>205</v>
+      </c>
       <c r="B206" t="s">
         <v>230</v>
       </c>
@@ -6571,7 +6870,10 @@
         <v>518</v>
       </c>
     </row>
-    <row r="207" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>206</v>
+      </c>
       <c r="B207" t="s">
         <v>521</v>
       </c>
@@ -6588,7 +6890,10 @@
         <v>520</v>
       </c>
     </row>
-    <row r="208" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>207</v>
+      </c>
       <c r="B208" t="s">
         <v>229</v>
       </c>
@@ -6605,7 +6910,10 @@
         <v>523</v>
       </c>
     </row>
-    <row r="209" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>208</v>
+      </c>
       <c r="B209" t="s">
         <v>525</v>
       </c>
@@ -6622,7 +6930,10 @@
         <v>526</v>
       </c>
     </row>
-    <row r="210" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>209</v>
+      </c>
       <c r="B210" t="s">
         <v>529</v>
       </c>
@@ -6639,7 +6950,10 @@
         <v>527</v>
       </c>
     </row>
-    <row r="211" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>210</v>
+      </c>
       <c r="B211" t="s">
         <v>230</v>
       </c>
@@ -6656,7 +6970,10 @@
         <v>531</v>
       </c>
     </row>
-    <row r="212" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>211</v>
+      </c>
       <c r="B212" t="s">
         <v>230</v>
       </c>
@@ -6673,7 +6990,10 @@
         <v>533</v>
       </c>
     </row>
-    <row r="213" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>212</v>
+      </c>
       <c r="B213" t="s">
         <v>230</v>
       </c>
@@ -6690,7 +7010,10 @@
         <v>535</v>
       </c>
     </row>
-    <row r="214" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>213</v>
+      </c>
       <c r="B214" t="s">
         <v>454</v>
       </c>
@@ -6707,7 +7030,10 @@
         <v>537</v>
       </c>
     </row>
-    <row r="215" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>214</v>
+      </c>
       <c r="B215" t="s">
         <v>230</v>
       </c>
@@ -6724,7 +7050,10 @@
         <v>539</v>
       </c>
     </row>
-    <row r="216" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>215</v>
+      </c>
       <c r="B216" t="s">
         <v>145</v>
       </c>
@@ -6741,7 +7070,10 @@
         <v>541</v>
       </c>
     </row>
-    <row r="217" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>216</v>
+      </c>
       <c r="B217" t="s">
         <v>488</v>
       </c>
@@ -6758,7 +7090,10 @@
         <v>543</v>
       </c>
     </row>
-    <row r="218" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>217</v>
+      </c>
       <c r="B218" t="s">
         <v>251</v>
       </c>
@@ -6775,7 +7110,10 @@
         <v>577</v>
       </c>
     </row>
-    <row r="219" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>218</v>
+      </c>
       <c r="B219" t="s">
         <v>580</v>
       </c>
@@ -6792,7 +7130,10 @@
         <v>579</v>
       </c>
     </row>
-    <row r="220" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>219</v>
+      </c>
       <c r="B220" t="s">
         <v>549</v>
       </c>
@@ -6809,7 +7150,10 @@
         <v>583</v>
       </c>
     </row>
-    <row r="221" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>220</v>
+      </c>
       <c r="B221" t="s">
         <v>145</v>
       </c>
@@ -6826,7 +7170,10 @@
         <v>586</v>
       </c>
     </row>
-    <row r="222" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>221</v>
+      </c>
       <c r="B222" t="s">
         <v>145</v>
       </c>
@@ -6843,7 +7190,10 @@
         <v>587</v>
       </c>
     </row>
-    <row r="223" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>222</v>
+      </c>
       <c r="B223" t="s">
         <v>591</v>
       </c>
@@ -6860,7 +7210,10 @@
         <v>592</v>
       </c>
     </row>
-    <row r="224" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>223</v>
+      </c>
       <c r="B224" t="s">
         <v>591</v>
       </c>
@@ -6877,7 +7230,10 @@
         <v>594</v>
       </c>
     </row>
-    <row r="225" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A225">
+        <v>224</v>
+      </c>
       <c r="B225" t="s">
         <v>548</v>
       </c>
@@ -6894,7 +7250,10 @@
         <v>595</v>
       </c>
     </row>
-    <row r="226" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A226">
+        <v>225</v>
+      </c>
       <c r="B226" t="s">
         <v>548</v>
       </c>
@@ -6911,7 +7270,10 @@
         <v>598</v>
       </c>
     </row>
-    <row r="227" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A227">
+        <v>226</v>
+      </c>
       <c r="B227" t="s">
         <v>602</v>
       </c>
@@ -6928,7 +7290,10 @@
         <v>605</v>
       </c>
     </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A228">
+        <v>227</v>
+      </c>
       <c r="B228" t="s">
         <v>272</v>
       </c>
@@ -6945,7 +7310,10 @@
         <v>607</v>
       </c>
     </row>
-    <row r="229" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>228</v>
+      </c>
       <c r="B229" t="s">
         <v>230</v>
       </c>
@@ -6962,7 +7330,10 @@
         <v>609</v>
       </c>
     </row>
-    <row r="230" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>229</v>
+      </c>
       <c r="B230" t="s">
         <v>580</v>
       </c>
@@ -6979,7 +7350,10 @@
         <v>612</v>
       </c>
     </row>
-    <row r="231" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A231">
+        <v>230</v>
+      </c>
       <c r="B231" t="s">
         <v>454</v>
       </c>
@@ -6996,7 +7370,10 @@
         <v>614</v>
       </c>
     </row>
-    <row r="232" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>231</v>
+      </c>
       <c r="B232" t="s">
         <v>615</v>
       </c>
@@ -7013,7 +7390,10 @@
         <v>617</v>
       </c>
     </row>
-    <row r="233" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>232</v>
+      </c>
       <c r="B233" t="s">
         <v>549</v>
       </c>
@@ -7030,7 +7410,10 @@
         <v>551</v>
       </c>
     </row>
-    <row r="234" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>233</v>
+      </c>
       <c r="B234" t="s">
         <v>548</v>
       </c>
@@ -7047,7 +7430,10 @@
         <v>553</v>
       </c>
     </row>
-    <row r="235" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>234</v>
+      </c>
       <c r="B235" t="s">
         <v>548</v>
       </c>
@@ -7064,7 +7450,10 @@
         <v>556</v>
       </c>
     </row>
-    <row r="236" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>235</v>
+      </c>
       <c r="B236" t="s">
         <v>549</v>
       </c>
@@ -7081,7 +7470,10 @@
         <v>558</v>
       </c>
     </row>
-    <row r="237" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A237">
+        <v>236</v>
+      </c>
       <c r="B237" t="s">
         <v>548</v>
       </c>
@@ -7098,7 +7490,10 @@
         <v>560</v>
       </c>
     </row>
-    <row r="238" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A238">
+        <v>237</v>
+      </c>
       <c r="B238" t="s">
         <v>562</v>
       </c>
@@ -7115,7 +7510,10 @@
         <v>563</v>
       </c>
     </row>
-    <row r="239" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A239">
+        <v>238</v>
+      </c>
       <c r="B239" t="s">
         <v>548</v>
       </c>
@@ -7132,7 +7530,10 @@
         <v>619</v>
       </c>
     </row>
-    <row r="240" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A240">
+        <v>239</v>
+      </c>
       <c r="B240" t="s">
         <v>620</v>
       </c>
@@ -7149,7 +7550,10 @@
         <v>624</v>
       </c>
     </row>
-    <row r="241" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A241">
+        <v>240</v>
+      </c>
       <c r="B241" t="s">
         <v>625</v>
       </c>
@@ -7166,7 +7570,10 @@
         <v>626</v>
       </c>
     </row>
-    <row r="242" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A242">
+        <v>241</v>
+      </c>
       <c r="B242" t="s">
         <v>625</v>
       </c>
@@ -7183,7 +7590,10 @@
         <v>629</v>
       </c>
     </row>
-    <row r="243" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A243">
+        <v>242</v>
+      </c>
       <c r="B243" t="s">
         <v>630</v>
       </c>
@@ -7200,7 +7610,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="244" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A244">
+        <v>243</v>
+      </c>
       <c r="B244" t="s">
         <v>230</v>
       </c>
@@ -7217,7 +7630,10 @@
         <v>642</v>
       </c>
     </row>
-    <row r="245" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A245">
+        <v>244</v>
+      </c>
       <c r="B245" t="s">
         <v>50</v>
       </c>
@@ -7234,7 +7650,10 @@
         <v>647</v>
       </c>
     </row>
-    <row r="246" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A246">
+        <v>245</v>
+      </c>
       <c r="B246" t="s">
         <v>230</v>
       </c>
@@ -7251,7 +7670,10 @@
         <v>650</v>
       </c>
     </row>
-    <row r="247" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A247">
+        <v>246</v>
+      </c>
       <c r="B247" t="s">
         <v>653</v>
       </c>
@@ -7268,7 +7690,10 @@
         <v>652</v>
       </c>
     </row>
-    <row r="248" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A248">
+        <v>247</v>
+      </c>
       <c r="B248" t="s">
         <v>653</v>
       </c>
@@ -7285,7 +7710,10 @@
         <v>654</v>
       </c>
     </row>
-    <row r="249" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A249">
+        <v>248</v>
+      </c>
       <c r="B249" t="s">
         <v>653</v>
       </c>
@@ -7302,7 +7730,10 @@
         <v>656</v>
       </c>
     </row>
-    <row r="250" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A250">
+        <v>249</v>
+      </c>
       <c r="B250" t="s">
         <v>653</v>
       </c>
@@ -7319,7 +7750,10 @@
         <v>657</v>
       </c>
     </row>
-    <row r="251" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A251">
+        <v>250</v>
+      </c>
       <c r="B251" t="s">
         <v>653</v>
       </c>
@@ -7336,7 +7770,10 @@
         <v>659</v>
       </c>
     </row>
-    <row r="252" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A252">
+        <v>251</v>
+      </c>
       <c r="B252" t="s">
         <v>653</v>
       </c>
@@ -7353,7 +7790,10 @@
         <v>660</v>
       </c>
     </row>
-    <row r="253" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A253">
+        <v>252</v>
+      </c>
       <c r="B253" t="s">
         <v>653</v>
       </c>
@@ -7370,7 +7810,10 @@
         <v>665</v>
       </c>
     </row>
-    <row r="254" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A254">
+        <v>253</v>
+      </c>
       <c r="B254" t="s">
         <v>653</v>
       </c>
@@ -7387,7 +7830,10 @@
         <v>667</v>
       </c>
     </row>
-    <row r="255" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A255">
+        <v>254</v>
+      </c>
       <c r="B255" t="s">
         <v>251</v>
       </c>
@@ -7404,7 +7850,10 @@
         <v>670</v>
       </c>
     </row>
-    <row r="256" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A256">
+        <v>255</v>
+      </c>
       <c r="B256" t="s">
         <v>454</v>
       </c>
@@ -7421,7 +7870,10 @@
         <v>672</v>
       </c>
     </row>
-    <row r="257" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A257">
+        <v>256</v>
+      </c>
       <c r="B257" t="s">
         <v>272</v>
       </c>
@@ -7438,7 +7890,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="258" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A258">
+        <v>257</v>
+      </c>
       <c r="B258" t="s">
         <v>272</v>
       </c>
@@ -7455,7 +7910,10 @@
         <v>678</v>
       </c>
     </row>
-    <row r="259" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A259">
+        <v>258</v>
+      </c>
       <c r="B259" t="s">
         <v>549</v>
       </c>
@@ -7472,7 +7930,10 @@
         <v>680</v>
       </c>
     </row>
-    <row r="260" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A260">
+        <v>259</v>
+      </c>
       <c r="B260" t="s">
         <v>682</v>
       </c>
@@ -7489,7 +7950,10 @@
         <v>684</v>
       </c>
     </row>
-    <row r="261" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A261">
+        <v>260</v>
+      </c>
       <c r="B261" t="s">
         <v>682</v>
       </c>
@@ -7506,7 +7970,10 @@
         <v>686</v>
       </c>
     </row>
-    <row r="262" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A262">
+        <v>261</v>
+      </c>
       <c r="B262" t="s">
         <v>230</v>
       </c>
@@ -7523,7 +7990,10 @@
         <v>609</v>
       </c>
     </row>
-    <row r="263" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A263">
+        <v>262</v>
+      </c>
       <c r="B263" t="s">
         <v>251</v>
       </c>
@@ -7540,7 +8010,10 @@
         <v>577</v>
       </c>
     </row>
-    <row r="264" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A264">
+        <v>263</v>
+      </c>
       <c r="B264" t="s">
         <v>229</v>
       </c>
@@ -7557,7 +8030,10 @@
         <v>689</v>
       </c>
     </row>
-    <row r="265" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A265">
+        <v>264</v>
+      </c>
       <c r="B265" t="s">
         <v>145</v>
       </c>
@@ -7574,7 +8050,10 @@
         <v>587</v>
       </c>
     </row>
-    <row r="266" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A266">
+        <v>265</v>
+      </c>
       <c r="B266" t="s">
         <v>548</v>
       </c>
@@ -7591,7 +8070,10 @@
         <v>692</v>
       </c>
     </row>
-    <row r="267" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A267">
+        <v>266</v>
+      </c>
       <c r="B267" t="s">
         <v>696</v>
       </c>
@@ -7608,7 +8090,10 @@
         <v>694</v>
       </c>
     </row>
-    <row r="268" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A268">
+        <v>267</v>
+      </c>
       <c r="B268" t="s">
         <v>696</v>
       </c>
@@ -7625,7 +8110,10 @@
         <v>697</v>
       </c>
     </row>
-    <row r="269" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A269">
+        <v>268</v>
+      </c>
       <c r="B269" t="s">
         <v>696</v>
       </c>
@@ -7642,7 +8130,10 @@
         <v>699</v>
       </c>
     </row>
-    <row r="270" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A270">
+        <v>269</v>
+      </c>
       <c r="B270" t="s">
         <v>696</v>
       </c>
@@ -7659,7 +8150,10 @@
         <v>701</v>
       </c>
     </row>
-    <row r="271" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A271">
+        <v>270</v>
+      </c>
       <c r="B271" t="s">
         <v>696</v>
       </c>
@@ -7676,7 +8170,10 @@
         <v>703</v>
       </c>
     </row>
-    <row r="272" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A272">
+        <v>271</v>
+      </c>
       <c r="B272" t="s">
         <v>696</v>
       </c>
@@ -7693,7 +8190,10 @@
         <v>705</v>
       </c>
     </row>
-    <row r="273" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A273">
+        <v>272</v>
+      </c>
       <c r="B273" t="s">
         <v>696</v>
       </c>
@@ -7710,7 +8210,10 @@
         <v>707</v>
       </c>
     </row>
-    <row r="274" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A274">
+        <v>273</v>
+      </c>
       <c r="B274" t="s">
         <v>696</v>
       </c>
@@ -7727,7 +8230,10 @@
         <v>709</v>
       </c>
     </row>
-    <row r="275" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A275">
+        <v>274</v>
+      </c>
       <c r="B275" t="s">
         <v>696</v>
       </c>
@@ -7744,7 +8250,10 @@
         <v>711</v>
       </c>
     </row>
-    <row r="276" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A276">
+        <v>275</v>
+      </c>
       <c r="B276" t="s">
         <v>625</v>
       </c>
@@ -7761,7 +8270,10 @@
         <v>714</v>
       </c>
     </row>
-    <row r="277" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A277">
+        <v>276</v>
+      </c>
       <c r="B277" t="s">
         <v>715</v>
       </c>
@@ -7778,7 +8290,10 @@
         <v>717</v>
       </c>
     </row>
-    <row r="278" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A278">
+        <v>277</v>
+      </c>
       <c r="B278" t="s">
         <v>720</v>
       </c>
@@ -7795,7 +8310,10 @@
         <v>719</v>
       </c>
     </row>
-    <row r="279" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A279">
+        <v>278</v>
+      </c>
       <c r="B279" t="s">
         <v>548</v>
       </c>
@@ -7812,7 +8330,10 @@
         <v>723</v>
       </c>
     </row>
-    <row r="280" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A280">
+        <v>279</v>
+      </c>
       <c r="B280" t="s">
         <v>251</v>
       </c>
@@ -7829,61 +8350,26 @@
         <v>724</v>
       </c>
     </row>
-    <row r="281" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="282" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="283" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="284" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="285" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="286" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="287" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="288" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="289" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="290" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="291" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="292" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="293" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="294" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="295" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="296" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="297" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="298" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="299" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="300" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="301" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="302" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="303" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="304" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="305" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="306" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="307" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="308" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="309" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="310" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="311" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="312" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="313" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="314" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="315" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="316" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="317" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="318" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="319" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="320" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="321" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="322" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="323" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="324" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="325" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="326" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="327" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="328" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="329" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="330" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="331" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="332" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="333" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="334" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="335" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A281">
+        <v>280</v>
+      </c>
+      <c r="B281" t="s">
+        <v>726</v>
+      </c>
+      <c r="C281" t="s">
+        <v>5</v>
+      </c>
+      <c r="D281" t="s">
+        <v>131</v>
+      </c>
+      <c r="E281" t="s">
+        <v>727</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>728</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{02761047-99F3-421A-BA67-554FF763D70E}"/>
@@ -8161,11 +8647,12 @@
     <hyperlink ref="F278" r:id="rId273" xr:uid="{B3BEAC81-90BF-42EC-99EB-2EFA3DF0832C}"/>
     <hyperlink ref="F279" r:id="rId274" xr:uid="{5B987029-66CC-4D09-83CE-FB98E8D38C22}"/>
     <hyperlink ref="F280" r:id="rId275" xr:uid="{5B19E107-4354-48AF-940B-5361100EB941}"/>
+    <hyperlink ref="F281" r:id="rId276" xr:uid="{52FC089E-1A61-4FCC-9E5D-8E711DD406FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId276"/>
+  <pageSetup orientation="portrait" r:id="rId277"/>
   <tableParts count="1">
-    <tablePart r:id="rId277"/>
+    <tablePart r:id="rId278"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -8176,17 +8663,17 @@
           </x14:formula1>
           <xm:sqref>C2:C335</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D8EBEEB8-B884-4C00-9B51-F5E336240EDE}">
-          <x14:formula1>
-            <xm:f>Values!$C$4:$C$39</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B335</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E9F62F5C-E13A-4017-8F5B-D791B22B6DC3}">
           <x14:formula1>
             <xm:f>Values!$E$4:$E$84</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D335</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D8EBEEB8-B884-4C00-9B51-F5E336240EDE}">
+          <x14:formula1>
+            <xm:f>Values!$C$4:$C$40</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B335</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8869,8 +9356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A6014D-2E27-4F54-8034-C9E495B040EE}">
   <dimension ref="C3:G84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9313,22 +9800,25 @@
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C38" s="5" t="s">
-        <v>315</v>
+      <c r="C38" t="s">
+        <v>726</v>
       </c>
       <c r="E38" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C39" t="s">
-        <v>50</v>
+      <c r="C39" s="5" t="s">
+        <v>315</v>
       </c>
       <c r="E39" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
       <c r="E40" t="s">
         <v>70</v>
       </c>

</xml_diff>